<commit_message>
add CISISTAG Condition Example
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-Condition-profile-Example.xlsx
+++ b/docs/StructureDefinition-Condition-profile-Example.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$135</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$129</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5037" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4816" uniqueCount="554">
   <si>
     <t>Property</t>
   </si>
@@ -39,13 +39,13 @@
     <t>Name</t>
   </si>
   <si>
-    <t>ConditionProfileExample</t>
+    <t>CISISTAGConditionProfile</t>
   </si>
   <si>
     <t>Title</t>
   </si>
   <si>
-    <t>03-Condition Profile(CISISTAG)</t>
+    <t>Condition Profile(CISISTAG)</t>
   </si>
   <si>
     <t>Status</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-07-31T21:33:26+08:00</t>
+    <t>2022-08-03T14:01:00+08:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -78,7 +78,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Example of a profile of Condition</t>
+    <t>Example of a profile of Condition(CISISTAG)</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -1372,13 +1372,145 @@
     <t>FiveWs.author</t>
   </si>
   <si>
-    <t>Condition.recorder.id</t>
-  </si>
-  <si>
-    <t>Condition.recorder.extension</t>
-  </si>
-  <si>
-    <t>Condition.recorder.reference</t>
+    <t>Condition.asserter</t>
+  </si>
+  <si>
+    <t>Person who asserts this condition</t>
+  </si>
+  <si>
+    <t>Individual who is making the condition statement.</t>
+  </si>
+  <si>
+    <t>REL-7.1 identifier + REL-7.12 type code</t>
+  </si>
+  <si>
+    <t>.participation[typeCode=INF].role</t>
+  </si>
+  <si>
+    <t>FiveWs.source</t>
+  </si>
+  <si>
+    <t>Condition.stage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BackboneElement
+</t>
+  </si>
+  <si>
+    <t>Stage/grade, usually assessed formally</t>
+  </si>
+  <si>
+    <t>Clinical stage or grade of a condition. May include formal severity assessments.</t>
+  </si>
+  <si>
+    <t>con-1:Stage SHALL have summary or assessment {summary.exists() or assessment.exists()}
+ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}</t>
+  </si>
+  <si>
+    <t>./inboundRelationship[typeCode=SUBJ].source[classCode=OBS, moodCode=EVN, code="stage/grade"]</t>
+  </si>
+  <si>
+    <t>Condition.stage.id</t>
+  </si>
+  <si>
+    <t>Condition.stage.extension</t>
+  </si>
+  <si>
+    <t>Condition.stage.modifierExtension</t>
+  </si>
+  <si>
+    <t>extensions
+user contentmodifiers</t>
+  </si>
+  <si>
+    <t>Extensions that cannot be ignored even if unrecognized</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element and that modifies the understanding of the element in which it is contained and/or the understanding of the containing element's descendants. Usually modifier elements provide negation or qualification. To make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.
+Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
+  </si>
+  <si>
+    <t>BackboneElement.modifierExtension</t>
+  </si>
+  <si>
+    <t>Condition.stage.summary</t>
+  </si>
+  <si>
+    <t>Simple summary (disease specific)</t>
+  </si>
+  <si>
+    <t>A simple summary of the stage such as "Stage 3". The determination of the stage is disease-specific.</t>
+  </si>
+  <si>
+    <t>Codes describing condition stages (e.g. Cancer stages).</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/condition-stage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">con-1
+</t>
+  </si>
+  <si>
+    <t>&lt; 254291000 |Staging and scales|</t>
+  </si>
+  <si>
+    <t>Condition.stage.summary.id</t>
+  </si>
+  <si>
+    <t>Condition.stage.summary.extension</t>
+  </si>
+  <si>
+    <t>Condition.stage.summary.coding</t>
+  </si>
+  <si>
+    <t>Condition.stage.summary.coding.id</t>
+  </si>
+  <si>
+    <t>Condition.stage.summary.coding.extension</t>
+  </si>
+  <si>
+    <t>Condition.stage.summary.coding.system</t>
+  </si>
+  <si>
+    <t>Condition.stage.summary.coding.version</t>
+  </si>
+  <si>
+    <t>Condition.stage.summary.coding.code</t>
+  </si>
+  <si>
+    <t>Condition.stage.summary.coding.display</t>
+  </si>
+  <si>
+    <t>Condition.stage.summary.coding.userSelected</t>
+  </si>
+  <si>
+    <t>Condition.stage.summary.text</t>
+  </si>
+  <si>
+    <t>Condition.stage.assessment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(ClinicalImpression|DiagnosticReport|Observation)
+</t>
+  </si>
+  <si>
+    <t>Formal record of assessment</t>
+  </si>
+  <si>
+    <t>Reference to a formal record of the evidence on which the staging assessment is based.</t>
+  </si>
+  <si>
+    <t>.self</t>
+  </si>
+  <si>
+    <t>Condition.stage.assessment.id</t>
+  </si>
+  <si>
+    <t>Condition.stage.assessment.extension</t>
+  </si>
+  <si>
+    <t>Condition.stage.assessment.reference</t>
   </si>
   <si>
     <t>Literal reference, Relative, internal or absolute URL</t>
@@ -1397,7 +1529,7 @@
 </t>
   </si>
   <si>
-    <t>Condition.recorder.type</t>
+    <t>Condition.stage.assessment.type</t>
   </si>
   <si>
     <t>Type the reference refers to (e.g. "Patient")</t>
@@ -1419,7 +1551,7 @@
     <t>Reference.type</t>
   </si>
   <si>
-    <t>Condition.recorder.identifier</t>
+    <t>Condition.stage.assessment.identifier</t>
   </si>
   <si>
     <t>Logical reference, when literal reference is not known</t>
@@ -1440,7 +1572,7 @@
     <t>.identifier</t>
   </si>
   <si>
-    <t>Condition.recorder.display</t>
+    <t>Condition.stage.assessment.display</t>
   </si>
   <si>
     <t>Text alternative for the resource</t>
@@ -1453,156 +1585,6 @@
   </si>
   <si>
     <t>Reference.display</t>
-  </si>
-  <si>
-    <t>Condition.asserter</t>
-  </si>
-  <si>
-    <t>Person who asserts this condition</t>
-  </si>
-  <si>
-    <t>Individual who is making the condition statement.</t>
-  </si>
-  <si>
-    <t>REL-7.1 identifier + REL-7.12 type code</t>
-  </si>
-  <si>
-    <t>.participation[typeCode=INF].role</t>
-  </si>
-  <si>
-    <t>FiveWs.source</t>
-  </si>
-  <si>
-    <t>Condition.stage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BackboneElement
-</t>
-  </si>
-  <si>
-    <t>Stage/grade, usually assessed formally</t>
-  </si>
-  <si>
-    <t>Clinical stage or grade of a condition. May include formal severity assessments.</t>
-  </si>
-  <si>
-    <t>con-1:Stage SHALL have summary or assessment {summary.exists() or assessment.exists()}
-ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}</t>
-  </si>
-  <si>
-    <t>./inboundRelationship[typeCode=SUBJ].source[classCode=OBS, moodCode=EVN, code="stage/grade"]</t>
-  </si>
-  <si>
-    <t>Condition.stage.id</t>
-  </si>
-  <si>
-    <t>Condition.stage.extension</t>
-  </si>
-  <si>
-    <t>Condition.stage.modifierExtension</t>
-  </si>
-  <si>
-    <t>extensions
-user contentmodifiers</t>
-  </si>
-  <si>
-    <t>Extensions that cannot be ignored even if unrecognized</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element and that modifies the understanding of the element in which it is contained and/or the understanding of the containing element's descendants. Usually modifier elements provide negation or qualification. To make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.
-Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
-  </si>
-  <si>
-    <t>BackboneElement.modifierExtension</t>
-  </si>
-  <si>
-    <t>Condition.stage.summary</t>
-  </si>
-  <si>
-    <t>Simple summary (disease specific)</t>
-  </si>
-  <si>
-    <t>A simple summary of the stage such as "Stage 3". The determination of the stage is disease-specific.</t>
-  </si>
-  <si>
-    <t>Codes describing condition stages (e.g. Cancer stages).</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/condition-stage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">con-1
-</t>
-  </si>
-  <si>
-    <t>&lt; 254291000 |Staging and scales|</t>
-  </si>
-  <si>
-    <t>Condition.stage.summary.id</t>
-  </si>
-  <si>
-    <t>Condition.stage.summary.extension</t>
-  </si>
-  <si>
-    <t>Condition.stage.summary.coding</t>
-  </si>
-  <si>
-    <t>Condition.stage.summary.coding.id</t>
-  </si>
-  <si>
-    <t>Condition.stage.summary.coding.extension</t>
-  </si>
-  <si>
-    <t>Condition.stage.summary.coding.system</t>
-  </si>
-  <si>
-    <t>Condition.stage.summary.coding.version</t>
-  </si>
-  <si>
-    <t>Condition.stage.summary.coding.code</t>
-  </si>
-  <si>
-    <t>Condition.stage.summary.coding.display</t>
-  </si>
-  <si>
-    <t>Condition.stage.summary.coding.userSelected</t>
-  </si>
-  <si>
-    <t>Condition.stage.summary.text</t>
-  </si>
-  <si>
-    <t>Condition.stage.assessment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(ClinicalImpression|DiagnosticReport|Observation)
-</t>
-  </si>
-  <si>
-    <t>Formal record of assessment</t>
-  </si>
-  <si>
-    <t>Reference to a formal record of the evidence on which the staging assessment is based.</t>
-  </si>
-  <si>
-    <t>.self</t>
-  </si>
-  <si>
-    <t>Condition.stage.assessment.id</t>
-  </si>
-  <si>
-    <t>Condition.stage.assessment.extension</t>
-  </si>
-  <si>
-    <t>Condition.stage.assessment.reference</t>
-  </si>
-  <si>
-    <t>Condition.stage.assessment.type</t>
-  </si>
-  <si>
-    <t>Condition.stage.assessment.identifier</t>
-  </si>
-  <si>
-    <t>Condition.stage.assessment.display</t>
   </si>
   <si>
     <t>Condition.stage.type</t>
@@ -2065,7 +2047,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO135"/>
+  <dimension ref="A1:AO129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -7166,7 +7148,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
         <v>312</v>
       </c>
@@ -7176,13 +7158,13 @@
       </c>
       <c r="D44" s="2"/>
       <c r="E44" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F44" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G44" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="H44" t="s" s="2">
         <v>76</v>
@@ -11751,7 +11733,7 @@
       </c>
       <c r="D83" s="2"/>
       <c r="E83" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F83" t="s" s="2">
         <v>87</v>
@@ -12100,7 +12082,7 @@
       </c>
       <c r="D86" s="2"/>
       <c r="E86" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F86" t="s" s="2">
         <v>87</v>
@@ -12227,16 +12209,16 @@
         <v>76</v>
       </c>
       <c r="I87" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="J87" t="s" s="2">
-        <v>89</v>
+        <v>432</v>
       </c>
       <c r="K87" t="s" s="2">
-        <v>154</v>
+        <v>438</v>
       </c>
       <c r="L87" t="s" s="2">
-        <v>155</v>
+        <v>439</v>
       </c>
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
@@ -12287,7 +12269,7 @@
         <v>76</v>
       </c>
       <c r="AE87" t="s" s="2">
-        <v>156</v>
+        <v>437</v>
       </c>
       <c r="AF87" t="s" s="2">
         <v>77</v>
@@ -12299,7 +12281,7 @@
         <v>76</v>
       </c>
       <c r="AI87" t="s" s="2">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="AJ87" t="s" s="2">
         <v>76</v>
@@ -12308,35 +12290,35 @@
         <v>76</v>
       </c>
       <c r="AL87" t="s" s="2">
-        <v>76</v>
+        <v>440</v>
       </c>
       <c r="AM87" t="s" s="2">
-        <v>157</v>
+        <v>441</v>
       </c>
       <c r="AN87" t="s" s="2">
-        <v>76</v>
+        <v>442</v>
       </c>
       <c r="AO87" t="s" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="88" hidden="true">
+    <row r="88">
       <c r="A88" t="s" s="2">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" t="s" s="2">
-        <v>132</v>
+        <v>76</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="F88" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G88" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="H88" t="s" s="2">
         <v>76</v>
@@ -12345,17 +12327,15 @@
         <v>76</v>
       </c>
       <c r="J88" t="s" s="2">
-        <v>133</v>
+        <v>444</v>
       </c>
       <c r="K88" t="s" s="2">
-        <v>134</v>
+        <v>445</v>
       </c>
       <c r="L88" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="M88" t="s" s="2">
-        <v>136</v>
-      </c>
+        <v>446</v>
+      </c>
+      <c r="M88" s="2"/>
       <c r="N88" s="2"/>
       <c r="O88" t="s" s="2">
         <v>76</v>
@@ -12392,19 +12372,19 @@
         <v>76</v>
       </c>
       <c r="AA88" t="s" s="2">
-        <v>160</v>
+        <v>76</v>
       </c>
       <c r="AB88" t="s" s="2">
-        <v>161</v>
+        <v>76</v>
       </c>
       <c r="AC88" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD88" t="s" s="2">
-        <v>162</v>
+        <v>76</v>
       </c>
       <c r="AE88" t="s" s="2">
-        <v>163</v>
+        <v>443</v>
       </c>
       <c r="AF88" t="s" s="2">
         <v>77</v>
@@ -12416,7 +12396,7 @@
         <v>76</v>
       </c>
       <c r="AI88" t="s" s="2">
-        <v>138</v>
+        <v>447</v>
       </c>
       <c r="AJ88" t="s" s="2">
         <v>76</v>
@@ -12428,7 +12408,7 @@
         <v>76</v>
       </c>
       <c r="AM88" t="s" s="2">
-        <v>157</v>
+        <v>448</v>
       </c>
       <c r="AN88" t="s" s="2">
         <v>76</v>
@@ -12439,7 +12419,7 @@
     </row>
     <row r="89" hidden="true">
       <c r="A89" t="s" s="2">
-        <v>439</v>
+        <v>449</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" t="s" s="2">
@@ -12447,7 +12427,7 @@
       </c>
       <c r="D89" s="2"/>
       <c r="E89" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F89" t="s" s="2">
         <v>87</v>
@@ -12459,20 +12439,18 @@
         <v>76</v>
       </c>
       <c r="I89" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="J89" t="s" s="2">
         <v>89</v>
       </c>
       <c r="K89" t="s" s="2">
-        <v>440</v>
+        <v>154</v>
       </c>
       <c r="L89" t="s" s="2">
-        <v>441</v>
-      </c>
-      <c r="M89" t="s" s="2">
-        <v>442</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="M89" s="2"/>
       <c r="N89" s="2"/>
       <c r="O89" t="s" s="2">
         <v>76</v>
@@ -12521,7 +12499,7 @@
         <v>76</v>
       </c>
       <c r="AE89" t="s" s="2">
-        <v>443</v>
+        <v>156</v>
       </c>
       <c r="AF89" t="s" s="2">
         <v>77</v>
@@ -12530,10 +12508,10 @@
         <v>87</v>
       </c>
       <c r="AH89" t="s" s="2">
-        <v>444</v>
+        <v>76</v>
       </c>
       <c r="AI89" t="s" s="2">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="AJ89" t="s" s="2">
         <v>76</v>
@@ -12545,7 +12523,7 @@
         <v>76</v>
       </c>
       <c r="AM89" t="s" s="2">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="AN89" t="s" s="2">
         <v>76</v>
@@ -12556,18 +12534,18 @@
     </row>
     <row r="90" hidden="true">
       <c r="A90" t="s" s="2">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" t="s" s="2">
-        <v>76</v>
+        <v>132</v>
       </c>
       <c r="D90" s="2"/>
       <c r="E90" t="s" s="2">
         <v>77</v>
       </c>
       <c r="F90" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G90" t="s" s="2">
         <v>76</v>
@@ -12576,19 +12554,19 @@
         <v>76</v>
       </c>
       <c r="I90" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="J90" t="s" s="2">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="K90" t="s" s="2">
-        <v>446</v>
+        <v>134</v>
       </c>
       <c r="L90" t="s" s="2">
-        <v>447</v>
+        <v>159</v>
       </c>
       <c r="M90" t="s" s="2">
-        <v>448</v>
+        <v>136</v>
       </c>
       <c r="N90" s="2"/>
       <c r="O90" t="s" s="2">
@@ -12614,13 +12592,13 @@
         <v>76</v>
       </c>
       <c r="W90" t="s" s="2">
-        <v>180</v>
+        <v>76</v>
       </c>
       <c r="X90" t="s" s="2">
-        <v>449</v>
+        <v>76</v>
       </c>
       <c r="Y90" t="s" s="2">
-        <v>450</v>
+        <v>76</v>
       </c>
       <c r="Z90" t="s" s="2">
         <v>76</v>
@@ -12638,19 +12616,19 @@
         <v>76</v>
       </c>
       <c r="AE90" t="s" s="2">
-        <v>451</v>
+        <v>163</v>
       </c>
       <c r="AF90" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG90" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AH90" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI90" t="s" s="2">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="AJ90" t="s" s="2">
         <v>76</v>
@@ -12662,7 +12640,7 @@
         <v>76</v>
       </c>
       <c r="AM90" t="s" s="2">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="AN90" t="s" s="2">
         <v>76</v>
@@ -12673,30 +12651,30 @@
     </row>
     <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" t="s" s="2">
-        <v>76</v>
+        <v>452</v>
       </c>
       <c r="D91" s="2"/>
       <c r="E91" t="s" s="2">
         <v>77</v>
       </c>
       <c r="F91" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G91" t="s" s="2">
         <v>76</v>
       </c>
       <c r="H91" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="I91" t="s" s="2">
         <v>88</v>
       </c>
       <c r="J91" t="s" s="2">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="K91" t="s" s="2">
         <v>453</v>
@@ -12705,9 +12683,11 @@
         <v>454</v>
       </c>
       <c r="M91" t="s" s="2">
-        <v>455</v>
-      </c>
-      <c r="N91" s="2"/>
+        <v>136</v>
+      </c>
+      <c r="N91" t="s" s="2">
+        <v>142</v>
+      </c>
       <c r="O91" t="s" s="2">
         <v>76</v>
       </c>
@@ -12755,19 +12735,19 @@
         <v>76</v>
       </c>
       <c r="AE91" t="s" s="2">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="AF91" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG91" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AH91" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI91" t="s" s="2">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="AJ91" t="s" s="2">
         <v>76</v>
@@ -12779,7 +12759,7 @@
         <v>76</v>
       </c>
       <c r="AM91" t="s" s="2">
-        <v>457</v>
+        <v>130</v>
       </c>
       <c r="AN91" t="s" s="2">
         <v>76</v>
@@ -12790,7 +12770,7 @@
     </row>
     <row r="92" hidden="true">
       <c r="A92" t="s" s="2">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" t="s" s="2">
@@ -12798,7 +12778,7 @@
       </c>
       <c r="D92" s="2"/>
       <c r="E92" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="F92" t="s" s="2">
         <v>87</v>
@@ -12810,20 +12790,18 @@
         <v>76</v>
       </c>
       <c r="I92" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="J92" t="s" s="2">
-        <v>89</v>
+        <v>175</v>
       </c>
       <c r="K92" t="s" s="2">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L92" t="s" s="2">
-        <v>460</v>
-      </c>
-      <c r="M92" t="s" s="2">
-        <v>461</v>
-      </c>
+        <v>458</v>
+      </c>
+      <c r="M92" s="2"/>
       <c r="N92" s="2"/>
       <c r="O92" t="s" s="2">
         <v>76</v>
@@ -12848,13 +12826,13 @@
         <v>76</v>
       </c>
       <c r="W92" t="s" s="2">
-        <v>76</v>
+        <v>348</v>
       </c>
       <c r="X92" t="s" s="2">
-        <v>76</v>
+        <v>459</v>
       </c>
       <c r="Y92" t="s" s="2">
-        <v>76</v>
+        <v>460</v>
       </c>
       <c r="Z92" t="s" s="2">
         <v>76</v>
@@ -12872,7 +12850,7 @@
         <v>76</v>
       </c>
       <c r="AE92" t="s" s="2">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="AF92" t="s" s="2">
         <v>77</v>
@@ -12881,7 +12859,7 @@
         <v>87</v>
       </c>
       <c r="AH92" t="s" s="2">
-        <v>76</v>
+        <v>461</v>
       </c>
       <c r="AI92" t="s" s="2">
         <v>99</v>
@@ -12890,13 +12868,13 @@
         <v>76</v>
       </c>
       <c r="AK92" t="s" s="2">
-        <v>76</v>
+        <v>462</v>
       </c>
       <c r="AL92" t="s" s="2">
-        <v>76</v>
+        <v>226</v>
       </c>
       <c r="AM92" t="s" s="2">
-        <v>130</v>
+        <v>354</v>
       </c>
       <c r="AN92" t="s" s="2">
         <v>76</v>
@@ -12927,16 +12905,16 @@
         <v>76</v>
       </c>
       <c r="I93" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="J93" t="s" s="2">
-        <v>432</v>
+        <v>89</v>
       </c>
       <c r="K93" t="s" s="2">
-        <v>464</v>
+        <v>154</v>
       </c>
       <c r="L93" t="s" s="2">
-        <v>465</v>
+        <v>155</v>
       </c>
       <c r="M93" s="2"/>
       <c r="N93" s="2"/>
@@ -12987,7 +12965,7 @@
         <v>76</v>
       </c>
       <c r="AE93" t="s" s="2">
-        <v>463</v>
+        <v>156</v>
       </c>
       <c r="AF93" t="s" s="2">
         <v>77</v>
@@ -12999,7 +12977,7 @@
         <v>76</v>
       </c>
       <c r="AI93" t="s" s="2">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="AJ93" t="s" s="2">
         <v>76</v>
@@ -13008,35 +12986,35 @@
         <v>76</v>
       </c>
       <c r="AL93" t="s" s="2">
-        <v>466</v>
+        <v>76</v>
       </c>
       <c r="AM93" t="s" s="2">
-        <v>467</v>
+        <v>157</v>
       </c>
       <c r="AN93" t="s" s="2">
-        <v>468</v>
+        <v>76</v>
       </c>
       <c r="AO93" t="s" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" hidden="true">
       <c r="A94" t="s" s="2">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" t="s" s="2">
-        <v>76</v>
+        <v>132</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F94" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G94" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="H94" t="s" s="2">
         <v>76</v>
@@ -13045,15 +13023,17 @@
         <v>76</v>
       </c>
       <c r="J94" t="s" s="2">
-        <v>470</v>
+        <v>133</v>
       </c>
       <c r="K94" t="s" s="2">
-        <v>471</v>
+        <v>134</v>
       </c>
       <c r="L94" t="s" s="2">
-        <v>472</v>
-      </c>
-      <c r="M94" s="2"/>
+        <v>159</v>
+      </c>
+      <c r="M94" t="s" s="2">
+        <v>136</v>
+      </c>
       <c r="N94" s="2"/>
       <c r="O94" t="s" s="2">
         <v>76</v>
@@ -13090,19 +13070,19 @@
         <v>76</v>
       </c>
       <c r="AA94" t="s" s="2">
-        <v>76</v>
+        <v>160</v>
       </c>
       <c r="AB94" t="s" s="2">
-        <v>76</v>
+        <v>161</v>
       </c>
       <c r="AC94" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD94" t="s" s="2">
-        <v>76</v>
+        <v>162</v>
       </c>
       <c r="AE94" t="s" s="2">
-        <v>469</v>
+        <v>163</v>
       </c>
       <c r="AF94" t="s" s="2">
         <v>77</v>
@@ -13114,7 +13094,7 @@
         <v>76</v>
       </c>
       <c r="AI94" t="s" s="2">
-        <v>473</v>
+        <v>138</v>
       </c>
       <c r="AJ94" t="s" s="2">
         <v>76</v>
@@ -13126,7 +13106,7 @@
         <v>76</v>
       </c>
       <c r="AM94" t="s" s="2">
-        <v>474</v>
+        <v>157</v>
       </c>
       <c r="AN94" t="s" s="2">
         <v>76</v>
@@ -13137,7 +13117,7 @@
     </row>
     <row r="95" hidden="true">
       <c r="A95" t="s" s="2">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" t="s" s="2">
@@ -13145,10 +13125,10 @@
       </c>
       <c r="D95" s="2"/>
       <c r="E95" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="F95" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G95" t="s" s="2">
         <v>76</v>
@@ -13157,19 +13137,23 @@
         <v>76</v>
       </c>
       <c r="I95" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="J95" t="s" s="2">
-        <v>89</v>
+        <v>232</v>
       </c>
       <c r="K95" t="s" s="2">
-        <v>154</v>
+        <v>233</v>
       </c>
       <c r="L95" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="M95" s="2"/>
-      <c r="N95" s="2"/>
+        <v>234</v>
+      </c>
+      <c r="M95" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="N95" t="s" s="2">
+        <v>236</v>
+      </c>
       <c r="O95" t="s" s="2">
         <v>76</v>
       </c>
@@ -13217,19 +13201,19 @@
         <v>76</v>
       </c>
       <c r="AE95" t="s" s="2">
-        <v>156</v>
+        <v>237</v>
       </c>
       <c r="AF95" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG95" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AH95" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI95" t="s" s="2">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="AJ95" t="s" s="2">
         <v>76</v>
@@ -13238,10 +13222,10 @@
         <v>76</v>
       </c>
       <c r="AL95" t="s" s="2">
-        <v>76</v>
+        <v>238</v>
       </c>
       <c r="AM95" t="s" s="2">
-        <v>157</v>
+        <v>239</v>
       </c>
       <c r="AN95" t="s" s="2">
         <v>76</v>
@@ -13252,18 +13236,18 @@
     </row>
     <row r="96" hidden="true">
       <c r="A96" t="s" s="2">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" t="s" s="2">
-        <v>132</v>
+        <v>76</v>
       </c>
       <c r="D96" s="2"/>
       <c r="E96" t="s" s="2">
         <v>77</v>
       </c>
       <c r="F96" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="G96" t="s" s="2">
         <v>76</v>
@@ -13275,17 +13259,15 @@
         <v>76</v>
       </c>
       <c r="J96" t="s" s="2">
-        <v>133</v>
+        <v>89</v>
       </c>
       <c r="K96" t="s" s="2">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="L96" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="M96" t="s" s="2">
-        <v>136</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="M96" s="2"/>
       <c r="N96" s="2"/>
       <c r="O96" t="s" s="2">
         <v>76</v>
@@ -13334,19 +13316,19 @@
         <v>76</v>
       </c>
       <c r="AE96" t="s" s="2">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="AF96" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG96" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="AH96" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI96" t="s" s="2">
-        <v>138</v>
+        <v>76</v>
       </c>
       <c r="AJ96" t="s" s="2">
         <v>76</v>
@@ -13369,11 +13351,11 @@
     </row>
     <row r="97" hidden="true">
       <c r="A97" t="s" s="2">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" t="s" s="2">
-        <v>478</v>
+        <v>132</v>
       </c>
       <c r="D97" s="2"/>
       <c r="E97" t="s" s="2">
@@ -13386,26 +13368,24 @@
         <v>76</v>
       </c>
       <c r="H97" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="I97" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="J97" t="s" s="2">
         <v>133</v>
       </c>
       <c r="K97" t="s" s="2">
-        <v>479</v>
+        <v>134</v>
       </c>
       <c r="L97" t="s" s="2">
-        <v>480</v>
+        <v>159</v>
       </c>
       <c r="M97" t="s" s="2">
         <v>136</v>
       </c>
-      <c r="N97" t="s" s="2">
-        <v>142</v>
-      </c>
+      <c r="N97" s="2"/>
       <c r="O97" t="s" s="2">
         <v>76</v>
       </c>
@@ -13441,19 +13421,19 @@
         <v>76</v>
       </c>
       <c r="AA97" t="s" s="2">
-        <v>76</v>
+        <v>160</v>
       </c>
       <c r="AB97" t="s" s="2">
-        <v>76</v>
+        <v>161</v>
       </c>
       <c r="AC97" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD97" t="s" s="2">
-        <v>76</v>
+        <v>162</v>
       </c>
       <c r="AE97" t="s" s="2">
-        <v>481</v>
+        <v>163</v>
       </c>
       <c r="AF97" t="s" s="2">
         <v>77</v>
@@ -13477,7 +13457,7 @@
         <v>76</v>
       </c>
       <c r="AM97" t="s" s="2">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="AN97" t="s" s="2">
         <v>76</v>
@@ -13488,7 +13468,7 @@
     </row>
     <row r="98" hidden="true">
       <c r="A98" t="s" s="2">
-        <v>482</v>
+        <v>468</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" t="s" s="2">
@@ -13508,25 +13488,29 @@
         <v>76</v>
       </c>
       <c r="I98" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="J98" t="s" s="2">
-        <v>175</v>
+        <v>101</v>
       </c>
       <c r="K98" t="s" s="2">
-        <v>483</v>
+        <v>243</v>
       </c>
       <c r="L98" t="s" s="2">
-        <v>484</v>
-      </c>
-      <c r="M98" s="2"/>
-      <c r="N98" s="2"/>
+        <v>244</v>
+      </c>
+      <c r="M98" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="N98" t="s" s="2">
+        <v>246</v>
+      </c>
       <c r="O98" t="s" s="2">
         <v>76</v>
       </c>
       <c r="P98" s="2"/>
       <c r="Q98" t="s" s="2">
-        <v>76</v>
+        <v>383</v>
       </c>
       <c r="R98" t="s" s="2">
         <v>76</v>
@@ -13544,13 +13528,13 @@
         <v>76</v>
       </c>
       <c r="W98" t="s" s="2">
-        <v>348</v>
+        <v>76</v>
       </c>
       <c r="X98" t="s" s="2">
-        <v>485</v>
+        <v>76</v>
       </c>
       <c r="Y98" t="s" s="2">
-        <v>486</v>
+        <v>76</v>
       </c>
       <c r="Z98" t="s" s="2">
         <v>76</v>
@@ -13568,7 +13552,7 @@
         <v>76</v>
       </c>
       <c r="AE98" t="s" s="2">
-        <v>482</v>
+        <v>248</v>
       </c>
       <c r="AF98" t="s" s="2">
         <v>77</v>
@@ -13577,7 +13561,7 @@
         <v>87</v>
       </c>
       <c r="AH98" t="s" s="2">
-        <v>487</v>
+        <v>76</v>
       </c>
       <c r="AI98" t="s" s="2">
         <v>99</v>
@@ -13586,13 +13570,13 @@
         <v>76</v>
       </c>
       <c r="AK98" t="s" s="2">
-        <v>488</v>
+        <v>76</v>
       </c>
       <c r="AL98" t="s" s="2">
-        <v>226</v>
+        <v>249</v>
       </c>
       <c r="AM98" t="s" s="2">
-        <v>354</v>
+        <v>250</v>
       </c>
       <c r="AN98" t="s" s="2">
         <v>76</v>
@@ -13603,7 +13587,7 @@
     </row>
     <row r="99" hidden="true">
       <c r="A99" t="s" s="2">
-        <v>489</v>
+        <v>469</v>
       </c>
       <c r="B99" s="2"/>
       <c r="C99" t="s" s="2">
@@ -13623,18 +13607,20 @@
         <v>76</v>
       </c>
       <c r="I99" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="J99" t="s" s="2">
         <v>89</v>
       </c>
       <c r="K99" t="s" s="2">
-        <v>154</v>
+        <v>252</v>
       </c>
       <c r="L99" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="M99" s="2"/>
+        <v>253</v>
+      </c>
+      <c r="M99" t="s" s="2">
+        <v>254</v>
+      </c>
       <c r="N99" s="2"/>
       <c r="O99" t="s" s="2">
         <v>76</v>
@@ -13683,7 +13669,7 @@
         <v>76</v>
       </c>
       <c r="AE99" t="s" s="2">
-        <v>156</v>
+        <v>255</v>
       </c>
       <c r="AF99" t="s" s="2">
         <v>77</v>
@@ -13695,7 +13681,7 @@
         <v>76</v>
       </c>
       <c r="AI99" t="s" s="2">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="AJ99" t="s" s="2">
         <v>76</v>
@@ -13704,10 +13690,10 @@
         <v>76</v>
       </c>
       <c r="AL99" t="s" s="2">
-        <v>76</v>
+        <v>256</v>
       </c>
       <c r="AM99" t="s" s="2">
-        <v>157</v>
+        <v>257</v>
       </c>
       <c r="AN99" t="s" s="2">
         <v>76</v>
@@ -13718,18 +13704,18 @@
     </row>
     <row r="100" hidden="true">
       <c r="A100" t="s" s="2">
-        <v>490</v>
+        <v>470</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" t="s" s="2">
-        <v>132</v>
+        <v>76</v>
       </c>
       <c r="D100" s="2"/>
       <c r="E100" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="F100" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="G100" t="s" s="2">
         <v>76</v>
@@ -13738,21 +13724,21 @@
         <v>76</v>
       </c>
       <c r="I100" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="J100" t="s" s="2">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="K100" t="s" s="2">
-        <v>134</v>
+        <v>259</v>
       </c>
       <c r="L100" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="M100" t="s" s="2">
-        <v>136</v>
-      </c>
-      <c r="N100" s="2"/>
+        <v>260</v>
+      </c>
+      <c r="M100" s="2"/>
+      <c r="N100" t="s" s="2">
+        <v>261</v>
+      </c>
       <c r="O100" t="s" s="2">
         <v>76</v>
       </c>
@@ -13788,31 +13774,31 @@
         <v>76</v>
       </c>
       <c r="AA100" t="s" s="2">
-        <v>160</v>
+        <v>76</v>
       </c>
       <c r="AB100" t="s" s="2">
-        <v>161</v>
+        <v>76</v>
       </c>
       <c r="AC100" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD100" t="s" s="2">
-        <v>162</v>
+        <v>76</v>
       </c>
       <c r="AE100" t="s" s="2">
-        <v>163</v>
+        <v>262</v>
       </c>
       <c r="AF100" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG100" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="AH100" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI100" t="s" s="2">
-        <v>138</v>
+        <v>99</v>
       </c>
       <c r="AJ100" t="s" s="2">
         <v>76</v>
@@ -13821,10 +13807,10 @@
         <v>76</v>
       </c>
       <c r="AL100" t="s" s="2">
-        <v>76</v>
+        <v>263</v>
       </c>
       <c r="AM100" t="s" s="2">
-        <v>157</v>
+        <v>264</v>
       </c>
       <c r="AN100" t="s" s="2">
         <v>76</v>
@@ -13835,7 +13821,7 @@
     </row>
     <row r="101" hidden="true">
       <c r="A101" t="s" s="2">
-        <v>491</v>
+        <v>471</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" t="s" s="2">
@@ -13846,7 +13832,7 @@
         <v>87</v>
       </c>
       <c r="F101" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="G101" t="s" s="2">
         <v>76</v>
@@ -13858,19 +13844,17 @@
         <v>88</v>
       </c>
       <c r="J101" t="s" s="2">
-        <v>232</v>
+        <v>89</v>
       </c>
       <c r="K101" t="s" s="2">
-        <v>233</v>
+        <v>266</v>
       </c>
       <c r="L101" t="s" s="2">
-        <v>234</v>
-      </c>
-      <c r="M101" t="s" s="2">
-        <v>235</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="M101" s="2"/>
       <c r="N101" t="s" s="2">
-        <v>236</v>
+        <v>268</v>
       </c>
       <c r="O101" t="s" s="2">
         <v>76</v>
@@ -13919,13 +13903,13 @@
         <v>76</v>
       </c>
       <c r="AE101" t="s" s="2">
-        <v>237</v>
+        <v>269</v>
       </c>
       <c r="AF101" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG101" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="AH101" t="s" s="2">
         <v>76</v>
@@ -13940,10 +13924,10 @@
         <v>76</v>
       </c>
       <c r="AL101" t="s" s="2">
-        <v>238</v>
+        <v>270</v>
       </c>
       <c r="AM101" t="s" s="2">
-        <v>239</v>
+        <v>271</v>
       </c>
       <c r="AN101" t="s" s="2">
         <v>76</v>
@@ -13954,7 +13938,7 @@
     </row>
     <row r="102" hidden="true">
       <c r="A102" t="s" s="2">
-        <v>492</v>
+        <v>472</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" t="s" s="2">
@@ -13974,19 +13958,23 @@
         <v>76</v>
       </c>
       <c r="I102" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="J102" t="s" s="2">
-        <v>89</v>
+        <v>273</v>
       </c>
       <c r="K102" t="s" s="2">
-        <v>154</v>
+        <v>274</v>
       </c>
       <c r="L102" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="M102" s="2"/>
-      <c r="N102" s="2"/>
+        <v>275</v>
+      </c>
+      <c r="M102" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="N102" t="s" s="2">
+        <v>277</v>
+      </c>
       <c r="O102" t="s" s="2">
         <v>76</v>
       </c>
@@ -14034,7 +14022,7 @@
         <v>76</v>
       </c>
       <c r="AE102" t="s" s="2">
-        <v>156</v>
+        <v>278</v>
       </c>
       <c r="AF102" t="s" s="2">
         <v>77</v>
@@ -14046,7 +14034,7 @@
         <v>76</v>
       </c>
       <c r="AI102" t="s" s="2">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="AJ102" t="s" s="2">
         <v>76</v>
@@ -14055,10 +14043,10 @@
         <v>76</v>
       </c>
       <c r="AL102" t="s" s="2">
-        <v>76</v>
+        <v>279</v>
       </c>
       <c r="AM102" t="s" s="2">
-        <v>157</v>
+        <v>280</v>
       </c>
       <c r="AN102" t="s" s="2">
         <v>76</v>
@@ -14069,18 +14057,18 @@
     </row>
     <row r="103" hidden="true">
       <c r="A103" t="s" s="2">
-        <v>493</v>
+        <v>473</v>
       </c>
       <c r="B103" s="2"/>
       <c r="C103" t="s" s="2">
-        <v>132</v>
+        <v>76</v>
       </c>
       <c r="D103" s="2"/>
       <c r="E103" t="s" s="2">
         <v>77</v>
       </c>
       <c r="F103" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="G103" t="s" s="2">
         <v>76</v>
@@ -14089,21 +14077,23 @@
         <v>76</v>
       </c>
       <c r="I103" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="J103" t="s" s="2">
-        <v>133</v>
+        <v>89</v>
       </c>
       <c r="K103" t="s" s="2">
-        <v>134</v>
+        <v>282</v>
       </c>
       <c r="L103" t="s" s="2">
-        <v>159</v>
+        <v>283</v>
       </c>
       <c r="M103" t="s" s="2">
-        <v>136</v>
-      </c>
-      <c r="N103" s="2"/>
+        <v>284</v>
+      </c>
+      <c r="N103" t="s" s="2">
+        <v>285</v>
+      </c>
       <c r="O103" t="s" s="2">
         <v>76</v>
       </c>
@@ -14139,31 +14129,31 @@
         <v>76</v>
       </c>
       <c r="AA103" t="s" s="2">
-        <v>160</v>
+        <v>76</v>
       </c>
       <c r="AB103" t="s" s="2">
-        <v>161</v>
+        <v>76</v>
       </c>
       <c r="AC103" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD103" t="s" s="2">
-        <v>162</v>
+        <v>76</v>
       </c>
       <c r="AE103" t="s" s="2">
-        <v>163</v>
+        <v>286</v>
       </c>
       <c r="AF103" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG103" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="AH103" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI103" t="s" s="2">
-        <v>138</v>
+        <v>99</v>
       </c>
       <c r="AJ103" t="s" s="2">
         <v>76</v>
@@ -14172,10 +14162,10 @@
         <v>76</v>
       </c>
       <c r="AL103" t="s" s="2">
-        <v>76</v>
+        <v>287</v>
       </c>
       <c r="AM103" t="s" s="2">
-        <v>157</v>
+        <v>288</v>
       </c>
       <c r="AN103" t="s" s="2">
         <v>76</v>
@@ -14186,7 +14176,7 @@
     </row>
     <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
-        <v>494</v>
+        <v>474</v>
       </c>
       <c r="B104" s="2"/>
       <c r="C104" t="s" s="2">
@@ -14194,10 +14184,10 @@
       </c>
       <c r="D104" s="2"/>
       <c r="E104" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F104" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G104" t="s" s="2">
         <v>76</v>
@@ -14206,23 +14196,19 @@
         <v>76</v>
       </c>
       <c r="I104" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="J104" t="s" s="2">
-        <v>101</v>
+        <v>475</v>
       </c>
       <c r="K104" t="s" s="2">
-        <v>243</v>
+        <v>476</v>
       </c>
       <c r="L104" t="s" s="2">
-        <v>244</v>
-      </c>
-      <c r="M104" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="N104" t="s" s="2">
-        <v>246</v>
-      </c>
+        <v>477</v>
+      </c>
+      <c r="M104" s="2"/>
+      <c r="N104" s="2"/>
       <c r="O104" t="s" s="2">
         <v>76</v>
       </c>
@@ -14270,16 +14256,16 @@
         <v>76</v>
       </c>
       <c r="AE104" t="s" s="2">
-        <v>248</v>
+        <v>474</v>
       </c>
       <c r="AF104" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG104" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AH104" t="s" s="2">
-        <v>76</v>
+        <v>461</v>
       </c>
       <c r="AI104" t="s" s="2">
         <v>99</v>
@@ -14291,10 +14277,10 @@
         <v>76</v>
       </c>
       <c r="AL104" t="s" s="2">
-        <v>249</v>
+        <v>76</v>
       </c>
       <c r="AM104" t="s" s="2">
-        <v>250</v>
+        <v>478</v>
       </c>
       <c r="AN104" t="s" s="2">
         <v>76</v>
@@ -14305,7 +14291,7 @@
     </row>
     <row r="105" hidden="true">
       <c r="A105" t="s" s="2">
-        <v>495</v>
+        <v>479</v>
       </c>
       <c r="B105" s="2"/>
       <c r="C105" t="s" s="2">
@@ -14325,20 +14311,18 @@
         <v>76</v>
       </c>
       <c r="I105" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="J105" t="s" s="2">
         <v>89</v>
       </c>
       <c r="K105" t="s" s="2">
-        <v>252</v>
+        <v>154</v>
       </c>
       <c r="L105" t="s" s="2">
-        <v>253</v>
-      </c>
-      <c r="M105" t="s" s="2">
-        <v>254</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="M105" s="2"/>
       <c r="N105" s="2"/>
       <c r="O105" t="s" s="2">
         <v>76</v>
@@ -14387,7 +14371,7 @@
         <v>76</v>
       </c>
       <c r="AE105" t="s" s="2">
-        <v>255</v>
+        <v>156</v>
       </c>
       <c r="AF105" t="s" s="2">
         <v>77</v>
@@ -14399,7 +14383,7 @@
         <v>76</v>
       </c>
       <c r="AI105" t="s" s="2">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="AJ105" t="s" s="2">
         <v>76</v>
@@ -14408,10 +14392,10 @@
         <v>76</v>
       </c>
       <c r="AL105" t="s" s="2">
-        <v>256</v>
+        <v>76</v>
       </c>
       <c r="AM105" t="s" s="2">
-        <v>257</v>
+        <v>157</v>
       </c>
       <c r="AN105" t="s" s="2">
         <v>76</v>
@@ -14422,18 +14406,18 @@
     </row>
     <row r="106" hidden="true">
       <c r="A106" t="s" s="2">
-        <v>496</v>
+        <v>480</v>
       </c>
       <c r="B106" s="2"/>
       <c r="C106" t="s" s="2">
-        <v>76</v>
+        <v>132</v>
       </c>
       <c r="D106" s="2"/>
       <c r="E106" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F106" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G106" t="s" s="2">
         <v>76</v>
@@ -14442,21 +14426,21 @@
         <v>76</v>
       </c>
       <c r="I106" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="J106" t="s" s="2">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="K106" t="s" s="2">
-        <v>259</v>
+        <v>134</v>
       </c>
       <c r="L106" t="s" s="2">
-        <v>260</v>
-      </c>
-      <c r="M106" s="2"/>
-      <c r="N106" t="s" s="2">
-        <v>261</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="M106" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="N106" s="2"/>
       <c r="O106" t="s" s="2">
         <v>76</v>
       </c>
@@ -14492,31 +14476,31 @@
         <v>76</v>
       </c>
       <c r="AA106" t="s" s="2">
-        <v>76</v>
+        <v>160</v>
       </c>
       <c r="AB106" t="s" s="2">
-        <v>76</v>
+        <v>161</v>
       </c>
       <c r="AC106" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD106" t="s" s="2">
-        <v>76</v>
+        <v>162</v>
       </c>
       <c r="AE106" t="s" s="2">
-        <v>262</v>
+        <v>163</v>
       </c>
       <c r="AF106" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG106" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AH106" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI106" t="s" s="2">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="AJ106" t="s" s="2">
         <v>76</v>
@@ -14525,10 +14509,10 @@
         <v>76</v>
       </c>
       <c r="AL106" t="s" s="2">
-        <v>263</v>
+        <v>76</v>
       </c>
       <c r="AM106" t="s" s="2">
-        <v>264</v>
+        <v>157</v>
       </c>
       <c r="AN106" t="s" s="2">
         <v>76</v>
@@ -14539,7 +14523,7 @@
     </row>
     <row r="107" hidden="true">
       <c r="A107" t="s" s="2">
-        <v>497</v>
+        <v>481</v>
       </c>
       <c r="B107" s="2"/>
       <c r="C107" t="s" s="2">
@@ -14565,15 +14549,15 @@
         <v>89</v>
       </c>
       <c r="K107" t="s" s="2">
-        <v>266</v>
+        <v>482</v>
       </c>
       <c r="L107" t="s" s="2">
-        <v>267</v>
-      </c>
-      <c r="M107" s="2"/>
-      <c r="N107" t="s" s="2">
-        <v>268</v>
-      </c>
+        <v>483</v>
+      </c>
+      <c r="M107" t="s" s="2">
+        <v>484</v>
+      </c>
+      <c r="N107" s="2"/>
       <c r="O107" t="s" s="2">
         <v>76</v>
       </c>
@@ -14621,7 +14605,7 @@
         <v>76</v>
       </c>
       <c r="AE107" t="s" s="2">
-        <v>269</v>
+        <v>485</v>
       </c>
       <c r="AF107" t="s" s="2">
         <v>77</v>
@@ -14630,7 +14614,7 @@
         <v>87</v>
       </c>
       <c r="AH107" t="s" s="2">
-        <v>76</v>
+        <v>486</v>
       </c>
       <c r="AI107" t="s" s="2">
         <v>99</v>
@@ -14642,10 +14626,10 @@
         <v>76</v>
       </c>
       <c r="AL107" t="s" s="2">
-        <v>270</v>
+        <v>76</v>
       </c>
       <c r="AM107" t="s" s="2">
-        <v>271</v>
+        <v>130</v>
       </c>
       <c r="AN107" t="s" s="2">
         <v>76</v>
@@ -14656,7 +14640,7 @@
     </row>
     <row r="108" hidden="true">
       <c r="A108" t="s" s="2">
-        <v>498</v>
+        <v>487</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" t="s" s="2">
@@ -14679,20 +14663,18 @@
         <v>88</v>
       </c>
       <c r="J108" t="s" s="2">
-        <v>273</v>
+        <v>101</v>
       </c>
       <c r="K108" t="s" s="2">
-        <v>274</v>
+        <v>488</v>
       </c>
       <c r="L108" t="s" s="2">
-        <v>275</v>
+        <v>489</v>
       </c>
       <c r="M108" t="s" s="2">
-        <v>276</v>
-      </c>
-      <c r="N108" t="s" s="2">
-        <v>277</v>
-      </c>
+        <v>490</v>
+      </c>
+      <c r="N108" s="2"/>
       <c r="O108" t="s" s="2">
         <v>76</v>
       </c>
@@ -14716,13 +14698,13 @@
         <v>76</v>
       </c>
       <c r="W108" t="s" s="2">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="X108" t="s" s="2">
-        <v>76</v>
+        <v>491</v>
       </c>
       <c r="Y108" t="s" s="2">
-        <v>76</v>
+        <v>492</v>
       </c>
       <c r="Z108" t="s" s="2">
         <v>76</v>
@@ -14740,7 +14722,7 @@
         <v>76</v>
       </c>
       <c r="AE108" t="s" s="2">
-        <v>278</v>
+        <v>493</v>
       </c>
       <c r="AF108" t="s" s="2">
         <v>77</v>
@@ -14761,10 +14743,10 @@
         <v>76</v>
       </c>
       <c r="AL108" t="s" s="2">
-        <v>279</v>
+        <v>76</v>
       </c>
       <c r="AM108" t="s" s="2">
-        <v>280</v>
+        <v>130</v>
       </c>
       <c r="AN108" t="s" s="2">
         <v>76</v>
@@ -14775,7 +14757,7 @@
     </row>
     <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="B109" s="2"/>
       <c r="C109" t="s" s="2">
@@ -14798,20 +14780,18 @@
         <v>88</v>
       </c>
       <c r="J109" t="s" s="2">
-        <v>89</v>
+        <v>145</v>
       </c>
       <c r="K109" t="s" s="2">
-        <v>282</v>
+        <v>495</v>
       </c>
       <c r="L109" t="s" s="2">
-        <v>283</v>
+        <v>496</v>
       </c>
       <c r="M109" t="s" s="2">
-        <v>284</v>
-      </c>
-      <c r="N109" t="s" s="2">
-        <v>285</v>
-      </c>
+        <v>497</v>
+      </c>
+      <c r="N109" s="2"/>
       <c r="O109" t="s" s="2">
         <v>76</v>
       </c>
@@ -14859,7 +14839,7 @@
         <v>76</v>
       </c>
       <c r="AE109" t="s" s="2">
-        <v>286</v>
+        <v>498</v>
       </c>
       <c r="AF109" t="s" s="2">
         <v>77</v>
@@ -14880,10 +14860,10 @@
         <v>76</v>
       </c>
       <c r="AL109" t="s" s="2">
-        <v>287</v>
+        <v>76</v>
       </c>
       <c r="AM109" t="s" s="2">
-        <v>288</v>
+        <v>499</v>
       </c>
       <c r="AN109" t="s" s="2">
         <v>76</v>
@@ -14902,10 +14882,10 @@
       </c>
       <c r="D110" s="2"/>
       <c r="E110" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F110" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="G110" t="s" s="2">
         <v>76</v>
@@ -14914,18 +14894,20 @@
         <v>76</v>
       </c>
       <c r="I110" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="J110" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="K110" t="s" s="2">
         <v>501</v>
       </c>
-      <c r="K110" t="s" s="2">
+      <c r="L110" t="s" s="2">
         <v>502</v>
       </c>
-      <c r="L110" t="s" s="2">
+      <c r="M110" t="s" s="2">
         <v>503</v>
       </c>
-      <c r="M110" s="2"/>
       <c r="N110" s="2"/>
       <c r="O110" t="s" s="2">
         <v>76</v>
@@ -14974,16 +14956,16 @@
         <v>76</v>
       </c>
       <c r="AE110" t="s" s="2">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="AF110" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG110" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="AH110" t="s" s="2">
-        <v>487</v>
+        <v>76</v>
       </c>
       <c r="AI110" t="s" s="2">
         <v>99</v>
@@ -14998,7 +14980,7 @@
         <v>76</v>
       </c>
       <c r="AM110" t="s" s="2">
-        <v>504</v>
+        <v>130</v>
       </c>
       <c r="AN110" t="s" s="2">
         <v>76</v>
@@ -15017,7 +14999,7 @@
       </c>
       <c r="D111" s="2"/>
       <c r="E111" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="F111" t="s" s="2">
         <v>87</v>
@@ -15032,13 +15014,13 @@
         <v>76</v>
       </c>
       <c r="J111" t="s" s="2">
-        <v>89</v>
+        <v>175</v>
       </c>
       <c r="K111" t="s" s="2">
-        <v>154</v>
+        <v>506</v>
       </c>
       <c r="L111" t="s" s="2">
-        <v>155</v>
+        <v>507</v>
       </c>
       <c r="M111" s="2"/>
       <c r="N111" s="2"/>
@@ -15065,13 +15047,13 @@
         <v>76</v>
       </c>
       <c r="W111" t="s" s="2">
-        <v>76</v>
+        <v>348</v>
       </c>
       <c r="X111" t="s" s="2">
-        <v>76</v>
+        <v>508</v>
       </c>
       <c r="Y111" t="s" s="2">
-        <v>76</v>
+        <v>509</v>
       </c>
       <c r="Z111" t="s" s="2">
         <v>76</v>
@@ -15089,7 +15071,7 @@
         <v>76</v>
       </c>
       <c r="AE111" t="s" s="2">
-        <v>156</v>
+        <v>505</v>
       </c>
       <c r="AF111" t="s" s="2">
         <v>77</v>
@@ -15101,7 +15083,7 @@
         <v>76</v>
       </c>
       <c r="AI111" t="s" s="2">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="AJ111" t="s" s="2">
         <v>76</v>
@@ -15113,7 +15095,7 @@
         <v>76</v>
       </c>
       <c r="AM111" t="s" s="2">
-        <v>157</v>
+        <v>510</v>
       </c>
       <c r="AN111" t="s" s="2">
         <v>76</v>
@@ -15124,18 +15106,18 @@
     </row>
     <row r="112" hidden="true">
       <c r="A112" t="s" s="2">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="B112" s="2"/>
       <c r="C112" t="s" s="2">
-        <v>132</v>
+        <v>76</v>
       </c>
       <c r="D112" s="2"/>
       <c r="E112" t="s" s="2">
         <v>77</v>
       </c>
       <c r="F112" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="G112" t="s" s="2">
         <v>76</v>
@@ -15147,17 +15129,15 @@
         <v>76</v>
       </c>
       <c r="J112" t="s" s="2">
-        <v>133</v>
+        <v>89</v>
       </c>
       <c r="K112" t="s" s="2">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="L112" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="M112" t="s" s="2">
-        <v>136</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="M112" s="2"/>
       <c r="N112" s="2"/>
       <c r="O112" t="s" s="2">
         <v>76</v>
@@ -15194,31 +15174,31 @@
         <v>76</v>
       </c>
       <c r="AA112" t="s" s="2">
-        <v>160</v>
+        <v>76</v>
       </c>
       <c r="AB112" t="s" s="2">
-        <v>161</v>
+        <v>76</v>
       </c>
       <c r="AC112" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD112" t="s" s="2">
-        <v>162</v>
+        <v>76</v>
       </c>
       <c r="AE112" t="s" s="2">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="AF112" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG112" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="AH112" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI112" t="s" s="2">
-        <v>138</v>
+        <v>76</v>
       </c>
       <c r="AJ112" t="s" s="2">
         <v>76</v>
@@ -15241,18 +15221,18 @@
     </row>
     <row r="113" hidden="true">
       <c r="A113" t="s" s="2">
-        <v>507</v>
+        <v>512</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" t="s" s="2">
-        <v>76</v>
+        <v>132</v>
       </c>
       <c r="D113" s="2"/>
       <c r="E113" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F113" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G113" t="s" s="2">
         <v>76</v>
@@ -15261,19 +15241,19 @@
         <v>76</v>
       </c>
       <c r="I113" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="J113" t="s" s="2">
-        <v>89</v>
+        <v>133</v>
       </c>
       <c r="K113" t="s" s="2">
-        <v>440</v>
+        <v>134</v>
       </c>
       <c r="L113" t="s" s="2">
-        <v>441</v>
+        <v>159</v>
       </c>
       <c r="M113" t="s" s="2">
-        <v>442</v>
+        <v>136</v>
       </c>
       <c r="N113" s="2"/>
       <c r="O113" t="s" s="2">
@@ -15311,31 +15291,31 @@
         <v>76</v>
       </c>
       <c r="AA113" t="s" s="2">
-        <v>76</v>
+        <v>160</v>
       </c>
       <c r="AB113" t="s" s="2">
-        <v>76</v>
+        <v>161</v>
       </c>
       <c r="AC113" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD113" t="s" s="2">
-        <v>76</v>
+        <v>162</v>
       </c>
       <c r="AE113" t="s" s="2">
-        <v>443</v>
+        <v>163</v>
       </c>
       <c r="AF113" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG113" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AH113" t="s" s="2">
-        <v>444</v>
+        <v>76</v>
       </c>
       <c r="AI113" t="s" s="2">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="AJ113" t="s" s="2">
         <v>76</v>
@@ -15347,7 +15327,7 @@
         <v>76</v>
       </c>
       <c r="AM113" t="s" s="2">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="AN113" t="s" s="2">
         <v>76</v>
@@ -15358,7 +15338,7 @@
     </row>
     <row r="114" hidden="true">
       <c r="A114" t="s" s="2">
-        <v>508</v>
+        <v>513</v>
       </c>
       <c r="B114" s="2"/>
       <c r="C114" t="s" s="2">
@@ -15366,10 +15346,10 @@
       </c>
       <c r="D114" s="2"/>
       <c r="E114" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="F114" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G114" t="s" s="2">
         <v>76</v>
@@ -15381,18 +15361,20 @@
         <v>88</v>
       </c>
       <c r="J114" t="s" s="2">
-        <v>101</v>
+        <v>232</v>
       </c>
       <c r="K114" t="s" s="2">
-        <v>446</v>
+        <v>233</v>
       </c>
       <c r="L114" t="s" s="2">
-        <v>447</v>
+        <v>234</v>
       </c>
       <c r="M114" t="s" s="2">
-        <v>448</v>
-      </c>
-      <c r="N114" s="2"/>
+        <v>235</v>
+      </c>
+      <c r="N114" t="s" s="2">
+        <v>236</v>
+      </c>
       <c r="O114" t="s" s="2">
         <v>76</v>
       </c>
@@ -15416,13 +15398,13 @@
         <v>76</v>
       </c>
       <c r="W114" t="s" s="2">
-        <v>180</v>
+        <v>76</v>
       </c>
       <c r="X114" t="s" s="2">
-        <v>449</v>
+        <v>76</v>
       </c>
       <c r="Y114" t="s" s="2">
-        <v>450</v>
+        <v>76</v>
       </c>
       <c r="Z114" t="s" s="2">
         <v>76</v>
@@ -15440,13 +15422,13 @@
         <v>76</v>
       </c>
       <c r="AE114" t="s" s="2">
-        <v>451</v>
+        <v>237</v>
       </c>
       <c r="AF114" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG114" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AH114" t="s" s="2">
         <v>76</v>
@@ -15461,10 +15443,10 @@
         <v>76</v>
       </c>
       <c r="AL114" t="s" s="2">
-        <v>76</v>
+        <v>238</v>
       </c>
       <c r="AM114" t="s" s="2">
-        <v>130</v>
+        <v>239</v>
       </c>
       <c r="AN114" t="s" s="2">
         <v>76</v>
@@ -15475,7 +15457,7 @@
     </row>
     <row r="115" hidden="true">
       <c r="A115" t="s" s="2">
-        <v>509</v>
+        <v>514</v>
       </c>
       <c r="B115" s="2"/>
       <c r="C115" t="s" s="2">
@@ -15495,20 +15477,18 @@
         <v>76</v>
       </c>
       <c r="I115" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="J115" t="s" s="2">
-        <v>145</v>
+        <v>89</v>
       </c>
       <c r="K115" t="s" s="2">
-        <v>453</v>
+        <v>154</v>
       </c>
       <c r="L115" t="s" s="2">
-        <v>454</v>
-      </c>
-      <c r="M115" t="s" s="2">
-        <v>455</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="M115" s="2"/>
       <c r="N115" s="2"/>
       <c r="O115" t="s" s="2">
         <v>76</v>
@@ -15557,7 +15537,7 @@
         <v>76</v>
       </c>
       <c r="AE115" t="s" s="2">
-        <v>456</v>
+        <v>156</v>
       </c>
       <c r="AF115" t="s" s="2">
         <v>77</v>
@@ -15569,7 +15549,7 @@
         <v>76</v>
       </c>
       <c r="AI115" t="s" s="2">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="AJ115" t="s" s="2">
         <v>76</v>
@@ -15581,7 +15561,7 @@
         <v>76</v>
       </c>
       <c r="AM115" t="s" s="2">
-        <v>457</v>
+        <v>157</v>
       </c>
       <c r="AN115" t="s" s="2">
         <v>76</v>
@@ -15592,18 +15572,18 @@
     </row>
     <row r="116" hidden="true">
       <c r="A116" t="s" s="2">
-        <v>510</v>
+        <v>515</v>
       </c>
       <c r="B116" s="2"/>
       <c r="C116" t="s" s="2">
-        <v>76</v>
+        <v>132</v>
       </c>
       <c r="D116" s="2"/>
       <c r="E116" t="s" s="2">
         <v>77</v>
       </c>
       <c r="F116" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G116" t="s" s="2">
         <v>76</v>
@@ -15612,19 +15592,19 @@
         <v>76</v>
       </c>
       <c r="I116" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="J116" t="s" s="2">
-        <v>89</v>
+        <v>133</v>
       </c>
       <c r="K116" t="s" s="2">
-        <v>459</v>
+        <v>134</v>
       </c>
       <c r="L116" t="s" s="2">
-        <v>460</v>
+        <v>159</v>
       </c>
       <c r="M116" t="s" s="2">
-        <v>461</v>
+        <v>136</v>
       </c>
       <c r="N116" s="2"/>
       <c r="O116" t="s" s="2">
@@ -15662,31 +15642,31 @@
         <v>76</v>
       </c>
       <c r="AA116" t="s" s="2">
-        <v>76</v>
+        <v>160</v>
       </c>
       <c r="AB116" t="s" s="2">
-        <v>76</v>
+        <v>161</v>
       </c>
       <c r="AC116" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD116" t="s" s="2">
-        <v>76</v>
+        <v>162</v>
       </c>
       <c r="AE116" t="s" s="2">
-        <v>462</v>
+        <v>163</v>
       </c>
       <c r="AF116" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG116" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AH116" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI116" t="s" s="2">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="AJ116" t="s" s="2">
         <v>76</v>
@@ -15698,7 +15678,7 @@
         <v>76</v>
       </c>
       <c r="AM116" t="s" s="2">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="AN116" t="s" s="2">
         <v>76</v>
@@ -15709,7 +15689,7 @@
     </row>
     <row r="117" hidden="true">
       <c r="A117" t="s" s="2">
-        <v>511</v>
+        <v>516</v>
       </c>
       <c r="B117" s="2"/>
       <c r="C117" t="s" s="2">
@@ -15729,25 +15709,29 @@
         <v>76</v>
       </c>
       <c r="I117" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="J117" t="s" s="2">
-        <v>175</v>
+        <v>101</v>
       </c>
       <c r="K117" t="s" s="2">
-        <v>512</v>
+        <v>243</v>
       </c>
       <c r="L117" t="s" s="2">
-        <v>513</v>
-      </c>
-      <c r="M117" s="2"/>
-      <c r="N117" s="2"/>
+        <v>244</v>
+      </c>
+      <c r="M117" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="N117" t="s" s="2">
+        <v>246</v>
+      </c>
       <c r="O117" t="s" s="2">
         <v>76</v>
       </c>
       <c r="P117" s="2"/>
       <c r="Q117" t="s" s="2">
-        <v>76</v>
+        <v>517</v>
       </c>
       <c r="R117" t="s" s="2">
         <v>76</v>
@@ -15765,13 +15749,13 @@
         <v>76</v>
       </c>
       <c r="W117" t="s" s="2">
-        <v>348</v>
+        <v>76</v>
       </c>
       <c r="X117" t="s" s="2">
-        <v>514</v>
+        <v>76</v>
       </c>
       <c r="Y117" t="s" s="2">
-        <v>515</v>
+        <v>76</v>
       </c>
       <c r="Z117" t="s" s="2">
         <v>76</v>
@@ -15789,7 +15773,7 @@
         <v>76</v>
       </c>
       <c r="AE117" t="s" s="2">
-        <v>511</v>
+        <v>248</v>
       </c>
       <c r="AF117" t="s" s="2">
         <v>77</v>
@@ -15810,10 +15794,10 @@
         <v>76</v>
       </c>
       <c r="AL117" t="s" s="2">
-        <v>76</v>
+        <v>249</v>
       </c>
       <c r="AM117" t="s" s="2">
-        <v>516</v>
+        <v>250</v>
       </c>
       <c r="AN117" t="s" s="2">
         <v>76</v>
@@ -15824,7 +15808,7 @@
     </row>
     <row r="118" hidden="true">
       <c r="A118" t="s" s="2">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B118" s="2"/>
       <c r="C118" t="s" s="2">
@@ -15844,18 +15828,20 @@
         <v>76</v>
       </c>
       <c r="I118" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="J118" t="s" s="2">
         <v>89</v>
       </c>
       <c r="K118" t="s" s="2">
-        <v>154</v>
+        <v>252</v>
       </c>
       <c r="L118" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="M118" s="2"/>
+        <v>253</v>
+      </c>
+      <c r="M118" t="s" s="2">
+        <v>254</v>
+      </c>
       <c r="N118" s="2"/>
       <c r="O118" t="s" s="2">
         <v>76</v>
@@ -15904,7 +15890,7 @@
         <v>76</v>
       </c>
       <c r="AE118" t="s" s="2">
-        <v>156</v>
+        <v>255</v>
       </c>
       <c r="AF118" t="s" s="2">
         <v>77</v>
@@ -15916,7 +15902,7 @@
         <v>76</v>
       </c>
       <c r="AI118" t="s" s="2">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="AJ118" t="s" s="2">
         <v>76</v>
@@ -15925,10 +15911,10 @@
         <v>76</v>
       </c>
       <c r="AL118" t="s" s="2">
-        <v>76</v>
+        <v>256</v>
       </c>
       <c r="AM118" t="s" s="2">
-        <v>157</v>
+        <v>257</v>
       </c>
       <c r="AN118" t="s" s="2">
         <v>76</v>
@@ -15939,18 +15925,18 @@
     </row>
     <row r="119" hidden="true">
       <c r="A119" t="s" s="2">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B119" s="2"/>
       <c r="C119" t="s" s="2">
-        <v>132</v>
+        <v>76</v>
       </c>
       <c r="D119" s="2"/>
       <c r="E119" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="F119" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="G119" t="s" s="2">
         <v>76</v>
@@ -15959,21 +15945,21 @@
         <v>76</v>
       </c>
       <c r="I119" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="J119" t="s" s="2">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="K119" t="s" s="2">
-        <v>134</v>
+        <v>259</v>
       </c>
       <c r="L119" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="M119" t="s" s="2">
-        <v>136</v>
-      </c>
-      <c r="N119" s="2"/>
+        <v>260</v>
+      </c>
+      <c r="M119" s="2"/>
+      <c r="N119" t="s" s="2">
+        <v>261</v>
+      </c>
       <c r="O119" t="s" s="2">
         <v>76</v>
       </c>
@@ -15982,7 +15968,7 @@
         <v>76</v>
       </c>
       <c r="R119" t="s" s="2">
-        <v>76</v>
+        <v>520</v>
       </c>
       <c r="S119" t="s" s="2">
         <v>76</v>
@@ -16009,31 +15995,31 @@
         <v>76</v>
       </c>
       <c r="AA119" t="s" s="2">
-        <v>160</v>
+        <v>76</v>
       </c>
       <c r="AB119" t="s" s="2">
-        <v>161</v>
+        <v>76</v>
       </c>
       <c r="AC119" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD119" t="s" s="2">
-        <v>162</v>
+        <v>76</v>
       </c>
       <c r="AE119" t="s" s="2">
-        <v>163</v>
+        <v>262</v>
       </c>
       <c r="AF119" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG119" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="AH119" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI119" t="s" s="2">
-        <v>138</v>
+        <v>99</v>
       </c>
       <c r="AJ119" t="s" s="2">
         <v>76</v>
@@ -16042,10 +16028,10 @@
         <v>76</v>
       </c>
       <c r="AL119" t="s" s="2">
-        <v>76</v>
+        <v>263</v>
       </c>
       <c r="AM119" t="s" s="2">
-        <v>157</v>
+        <v>264</v>
       </c>
       <c r="AN119" t="s" s="2">
         <v>76</v>
@@ -16056,7 +16042,7 @@
     </row>
     <row r="120" hidden="true">
       <c r="A120" t="s" s="2">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="B120" s="2"/>
       <c r="C120" t="s" s="2">
@@ -16067,7 +16053,7 @@
         <v>87</v>
       </c>
       <c r="F120" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="G120" t="s" s="2">
         <v>76</v>
@@ -16079,19 +16065,17 @@
         <v>88</v>
       </c>
       <c r="J120" t="s" s="2">
-        <v>232</v>
+        <v>89</v>
       </c>
       <c r="K120" t="s" s="2">
-        <v>233</v>
+        <v>266</v>
       </c>
       <c r="L120" t="s" s="2">
-        <v>234</v>
-      </c>
-      <c r="M120" t="s" s="2">
-        <v>235</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="M120" s="2"/>
       <c r="N120" t="s" s="2">
-        <v>236</v>
+        <v>268</v>
       </c>
       <c r="O120" t="s" s="2">
         <v>76</v>
@@ -16101,7 +16085,7 @@
         <v>76</v>
       </c>
       <c r="R120" t="s" s="2">
-        <v>76</v>
+        <v>522</v>
       </c>
       <c r="S120" t="s" s="2">
         <v>76</v>
@@ -16140,13 +16124,13 @@
         <v>76</v>
       </c>
       <c r="AE120" t="s" s="2">
-        <v>237</v>
+        <v>269</v>
       </c>
       <c r="AF120" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG120" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="AH120" t="s" s="2">
         <v>76</v>
@@ -16161,10 +16145,10 @@
         <v>76</v>
       </c>
       <c r="AL120" t="s" s="2">
-        <v>238</v>
+        <v>270</v>
       </c>
       <c r="AM120" t="s" s="2">
-        <v>239</v>
+        <v>271</v>
       </c>
       <c r="AN120" t="s" s="2">
         <v>76</v>
@@ -16175,7 +16159,7 @@
     </row>
     <row r="121" hidden="true">
       <c r="A121" t="s" s="2">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="B121" s="2"/>
       <c r="C121" t="s" s="2">
@@ -16195,19 +16179,23 @@
         <v>76</v>
       </c>
       <c r="I121" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="J121" t="s" s="2">
-        <v>89</v>
+        <v>273</v>
       </c>
       <c r="K121" t="s" s="2">
-        <v>154</v>
+        <v>274</v>
       </c>
       <c r="L121" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="M121" s="2"/>
-      <c r="N121" s="2"/>
+        <v>275</v>
+      </c>
+      <c r="M121" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="N121" t="s" s="2">
+        <v>277</v>
+      </c>
       <c r="O121" t="s" s="2">
         <v>76</v>
       </c>
@@ -16255,7 +16243,7 @@
         <v>76</v>
       </c>
       <c r="AE121" t="s" s="2">
-        <v>156</v>
+        <v>278</v>
       </c>
       <c r="AF121" t="s" s="2">
         <v>77</v>
@@ -16267,7 +16255,7 @@
         <v>76</v>
       </c>
       <c r="AI121" t="s" s="2">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="AJ121" t="s" s="2">
         <v>76</v>
@@ -16276,10 +16264,10 @@
         <v>76</v>
       </c>
       <c r="AL121" t="s" s="2">
-        <v>76</v>
+        <v>279</v>
       </c>
       <c r="AM121" t="s" s="2">
-        <v>157</v>
+        <v>280</v>
       </c>
       <c r="AN121" t="s" s="2">
         <v>76</v>
@@ -16290,18 +16278,18 @@
     </row>
     <row r="122" hidden="true">
       <c r="A122" t="s" s="2">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="B122" s="2"/>
       <c r="C122" t="s" s="2">
-        <v>132</v>
+        <v>76</v>
       </c>
       <c r="D122" s="2"/>
       <c r="E122" t="s" s="2">
         <v>77</v>
       </c>
       <c r="F122" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="G122" t="s" s="2">
         <v>76</v>
@@ -16310,21 +16298,23 @@
         <v>76</v>
       </c>
       <c r="I122" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="J122" t="s" s="2">
-        <v>133</v>
+        <v>89</v>
       </c>
       <c r="K122" t="s" s="2">
-        <v>134</v>
+        <v>282</v>
       </c>
       <c r="L122" t="s" s="2">
-        <v>159</v>
+        <v>283</v>
       </c>
       <c r="M122" t="s" s="2">
-        <v>136</v>
-      </c>
-      <c r="N122" s="2"/>
+        <v>284</v>
+      </c>
+      <c r="N122" t="s" s="2">
+        <v>285</v>
+      </c>
       <c r="O122" t="s" s="2">
         <v>76</v>
       </c>
@@ -16360,31 +16350,31 @@
         <v>76</v>
       </c>
       <c r="AA122" t="s" s="2">
-        <v>160</v>
+        <v>76</v>
       </c>
       <c r="AB122" t="s" s="2">
-        <v>161</v>
+        <v>76</v>
       </c>
       <c r="AC122" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD122" t="s" s="2">
-        <v>162</v>
+        <v>76</v>
       </c>
       <c r="AE122" t="s" s="2">
-        <v>163</v>
+        <v>286</v>
       </c>
       <c r="AF122" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG122" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="AH122" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI122" t="s" s="2">
-        <v>138</v>
+        <v>99</v>
       </c>
       <c r="AJ122" t="s" s="2">
         <v>76</v>
@@ -16393,10 +16383,10 @@
         <v>76</v>
       </c>
       <c r="AL122" t="s" s="2">
-        <v>76</v>
+        <v>287</v>
       </c>
       <c r="AM122" t="s" s="2">
-        <v>157</v>
+        <v>288</v>
       </c>
       <c r="AN122" t="s" s="2">
         <v>76</v>
@@ -16407,7 +16397,7 @@
     </row>
     <row r="123" hidden="true">
       <c r="A123" t="s" s="2">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="B123" s="2"/>
       <c r="C123" t="s" s="2">
@@ -16415,10 +16405,10 @@
       </c>
       <c r="D123" s="2"/>
       <c r="E123" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F123" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G123" t="s" s="2">
         <v>76</v>
@@ -16427,29 +16417,27 @@
         <v>76</v>
       </c>
       <c r="I123" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="J123" t="s" s="2">
-        <v>101</v>
+        <v>444</v>
       </c>
       <c r="K123" t="s" s="2">
-        <v>243</v>
+        <v>526</v>
       </c>
       <c r="L123" t="s" s="2">
-        <v>244</v>
+        <v>527</v>
       </c>
       <c r="M123" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="N123" t="s" s="2">
-        <v>246</v>
-      </c>
+        <v>528</v>
+      </c>
+      <c r="N123" s="2"/>
       <c r="O123" t="s" s="2">
         <v>76</v>
       </c>
       <c r="P123" s="2"/>
       <c r="Q123" t="s" s="2">
-        <v>523</v>
+        <v>76</v>
       </c>
       <c r="R123" t="s" s="2">
         <v>76</v>
@@ -16491,19 +16479,19 @@
         <v>76</v>
       </c>
       <c r="AE123" t="s" s="2">
-        <v>248</v>
+        <v>525</v>
       </c>
       <c r="AF123" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG123" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AH123" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI123" t="s" s="2">
-        <v>99</v>
+        <v>529</v>
       </c>
       <c r="AJ123" t="s" s="2">
         <v>76</v>
@@ -16512,10 +16500,10 @@
         <v>76</v>
       </c>
       <c r="AL123" t="s" s="2">
-        <v>249</v>
+        <v>76</v>
       </c>
       <c r="AM123" t="s" s="2">
-        <v>250</v>
+        <v>530</v>
       </c>
       <c r="AN123" t="s" s="2">
         <v>76</v>
@@ -16526,7 +16514,7 @@
     </row>
     <row r="124" hidden="true">
       <c r="A124" t="s" s="2">
-        <v>524</v>
+        <v>531</v>
       </c>
       <c r="B124" s="2"/>
       <c r="C124" t="s" s="2">
@@ -16546,20 +16534,18 @@
         <v>76</v>
       </c>
       <c r="I124" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="J124" t="s" s="2">
         <v>89</v>
       </c>
       <c r="K124" t="s" s="2">
-        <v>252</v>
+        <v>154</v>
       </c>
       <c r="L124" t="s" s="2">
-        <v>253</v>
-      </c>
-      <c r="M124" t="s" s="2">
-        <v>254</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="M124" s="2"/>
       <c r="N124" s="2"/>
       <c r="O124" t="s" s="2">
         <v>76</v>
@@ -16608,7 +16594,7 @@
         <v>76</v>
       </c>
       <c r="AE124" t="s" s="2">
-        <v>255</v>
+        <v>156</v>
       </c>
       <c r="AF124" t="s" s="2">
         <v>77</v>
@@ -16620,7 +16606,7 @@
         <v>76</v>
       </c>
       <c r="AI124" t="s" s="2">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="AJ124" t="s" s="2">
         <v>76</v>
@@ -16629,10 +16615,10 @@
         <v>76</v>
       </c>
       <c r="AL124" t="s" s="2">
-        <v>256</v>
+        <v>76</v>
       </c>
       <c r="AM124" t="s" s="2">
-        <v>257</v>
+        <v>157</v>
       </c>
       <c r="AN124" t="s" s="2">
         <v>76</v>
@@ -16643,18 +16629,18 @@
     </row>
     <row r="125" hidden="true">
       <c r="A125" t="s" s="2">
-        <v>525</v>
+        <v>532</v>
       </c>
       <c r="B125" s="2"/>
       <c r="C125" t="s" s="2">
-        <v>76</v>
+        <v>132</v>
       </c>
       <c r="D125" s="2"/>
       <c r="E125" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F125" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G125" t="s" s="2">
         <v>76</v>
@@ -16663,27 +16649,27 @@
         <v>76</v>
       </c>
       <c r="I125" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="J125" t="s" s="2">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="K125" t="s" s="2">
-        <v>259</v>
+        <v>134</v>
       </c>
       <c r="L125" t="s" s="2">
-        <v>260</v>
-      </c>
-      <c r="M125" s="2"/>
-      <c r="N125" t="s" s="2">
-        <v>261</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="M125" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="N125" s="2"/>
       <c r="O125" t="s" s="2">
         <v>76</v>
       </c>
       <c r="P125" s="2"/>
       <c r="Q125" t="s" s="2">
-        <v>526</v>
+        <v>76</v>
       </c>
       <c r="R125" t="s" s="2">
         <v>76</v>
@@ -16725,19 +16711,19 @@
         <v>76</v>
       </c>
       <c r="AE125" t="s" s="2">
-        <v>262</v>
+        <v>163</v>
       </c>
       <c r="AF125" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG125" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AH125" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI125" t="s" s="2">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="AJ125" t="s" s="2">
         <v>76</v>
@@ -16746,10 +16732,10 @@
         <v>76</v>
       </c>
       <c r="AL125" t="s" s="2">
-        <v>263</v>
+        <v>76</v>
       </c>
       <c r="AM125" t="s" s="2">
-        <v>264</v>
+        <v>157</v>
       </c>
       <c r="AN125" t="s" s="2">
         <v>76</v>
@@ -16760,47 +16746,49 @@
     </row>
     <row r="126" hidden="true">
       <c r="A126" t="s" s="2">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B126" s="2"/>
       <c r="C126" t="s" s="2">
-        <v>76</v>
+        <v>452</v>
       </c>
       <c r="D126" s="2"/>
       <c r="E126" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F126" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G126" t="s" s="2">
         <v>76</v>
       </c>
       <c r="H126" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="I126" t="s" s="2">
         <v>88</v>
       </c>
       <c r="J126" t="s" s="2">
-        <v>89</v>
+        <v>133</v>
       </c>
       <c r="K126" t="s" s="2">
-        <v>266</v>
+        <v>453</v>
       </c>
       <c r="L126" t="s" s="2">
-        <v>267</v>
-      </c>
-      <c r="M126" s="2"/>
+        <v>454</v>
+      </c>
+      <c r="M126" t="s" s="2">
+        <v>136</v>
+      </c>
       <c r="N126" t="s" s="2">
-        <v>268</v>
+        <v>142</v>
       </c>
       <c r="O126" t="s" s="2">
         <v>76</v>
       </c>
       <c r="P126" s="2"/>
       <c r="Q126" t="s" s="2">
-        <v>528</v>
+        <v>76</v>
       </c>
       <c r="R126" t="s" s="2">
         <v>76</v>
@@ -16842,19 +16830,19 @@
         <v>76</v>
       </c>
       <c r="AE126" t="s" s="2">
-        <v>269</v>
+        <v>455</v>
       </c>
       <c r="AF126" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG126" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AH126" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI126" t="s" s="2">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="AJ126" t="s" s="2">
         <v>76</v>
@@ -16863,10 +16851,10 @@
         <v>76</v>
       </c>
       <c r="AL126" t="s" s="2">
-        <v>270</v>
+        <v>76</v>
       </c>
       <c r="AM126" t="s" s="2">
-        <v>271</v>
+        <v>130</v>
       </c>
       <c r="AN126" t="s" s="2">
         <v>76</v>
@@ -16877,7 +16865,7 @@
     </row>
     <row r="127" hidden="true">
       <c r="A127" t="s" s="2">
-        <v>529</v>
+        <v>534</v>
       </c>
       <c r="B127" s="2"/>
       <c r="C127" t="s" s="2">
@@ -16888,7 +16876,7 @@
         <v>77</v>
       </c>
       <c r="F127" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G127" t="s" s="2">
         <v>76</v>
@@ -16900,20 +16888,16 @@
         <v>88</v>
       </c>
       <c r="J127" t="s" s="2">
-        <v>273</v>
+        <v>175</v>
       </c>
       <c r="K127" t="s" s="2">
-        <v>274</v>
+        <v>535</v>
       </c>
       <c r="L127" t="s" s="2">
-        <v>275</v>
-      </c>
-      <c r="M127" t="s" s="2">
-        <v>276</v>
-      </c>
-      <c r="N127" t="s" s="2">
-        <v>277</v>
-      </c>
+        <v>536</v>
+      </c>
+      <c r="M127" s="2"/>
+      <c r="N127" s="2"/>
       <c r="O127" t="s" s="2">
         <v>76</v>
       </c>
@@ -16937,13 +16921,13 @@
         <v>76</v>
       </c>
       <c r="W127" t="s" s="2">
-        <v>76</v>
+        <v>348</v>
       </c>
       <c r="X127" t="s" s="2">
-        <v>76</v>
+        <v>537</v>
       </c>
       <c r="Y127" t="s" s="2">
-        <v>76</v>
+        <v>538</v>
       </c>
       <c r="Z127" t="s" s="2">
         <v>76</v>
@@ -16961,34 +16945,34 @@
         <v>76</v>
       </c>
       <c r="AE127" t="s" s="2">
-        <v>278</v>
+        <v>534</v>
       </c>
       <c r="AF127" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG127" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AH127" t="s" s="2">
-        <v>76</v>
+        <v>539</v>
       </c>
       <c r="AI127" t="s" s="2">
         <v>99</v>
       </c>
       <c r="AJ127" t="s" s="2">
-        <v>76</v>
+        <v>540</v>
       </c>
       <c r="AK127" t="s" s="2">
-        <v>76</v>
+        <v>317</v>
       </c>
       <c r="AL127" t="s" s="2">
-        <v>279</v>
+        <v>76</v>
       </c>
       <c r="AM127" t="s" s="2">
-        <v>280</v>
+        <v>541</v>
       </c>
       <c r="AN127" t="s" s="2">
-        <v>76</v>
+        <v>542</v>
       </c>
       <c r="AO127" t="s" s="2">
         <v>76</v>
@@ -16996,7 +16980,7 @@
     </row>
     <row r="128" hidden="true">
       <c r="A128" t="s" s="2">
-        <v>530</v>
+        <v>543</v>
       </c>
       <c r="B128" s="2"/>
       <c r="C128" t="s" s="2">
@@ -17007,7 +16991,7 @@
         <v>77</v>
       </c>
       <c r="F128" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G128" t="s" s="2">
         <v>76</v>
@@ -17019,20 +17003,16 @@
         <v>88</v>
       </c>
       <c r="J128" t="s" s="2">
-        <v>89</v>
+        <v>544</v>
       </c>
       <c r="K128" t="s" s="2">
-        <v>282</v>
+        <v>545</v>
       </c>
       <c r="L128" t="s" s="2">
-        <v>283</v>
-      </c>
-      <c r="M128" t="s" s="2">
-        <v>284</v>
-      </c>
-      <c r="N128" t="s" s="2">
-        <v>285</v>
-      </c>
+        <v>546</v>
+      </c>
+      <c r="M128" s="2"/>
+      <c r="N128" s="2"/>
       <c r="O128" t="s" s="2">
         <v>76</v>
       </c>
@@ -17080,16 +17060,16 @@
         <v>76</v>
       </c>
       <c r="AE128" t="s" s="2">
-        <v>286</v>
+        <v>543</v>
       </c>
       <c r="AF128" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG128" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AH128" t="s" s="2">
-        <v>76</v>
+        <v>539</v>
       </c>
       <c r="AI128" t="s" s="2">
         <v>99</v>
@@ -17101,13 +17081,13 @@
         <v>76</v>
       </c>
       <c r="AL128" t="s" s="2">
-        <v>287</v>
+        <v>76</v>
       </c>
       <c r="AM128" t="s" s="2">
-        <v>288</v>
+        <v>478</v>
       </c>
       <c r="AN128" t="s" s="2">
-        <v>76</v>
+        <v>542</v>
       </c>
       <c r="AO128" t="s" s="2">
         <v>76</v>
@@ -17115,7 +17095,7 @@
     </row>
     <row r="129" hidden="true">
       <c r="A129" t="s" s="2">
-        <v>531</v>
+        <v>547</v>
       </c>
       <c r="B129" s="2"/>
       <c r="C129" t="s" s="2">
@@ -17138,17 +17118,15 @@
         <v>76</v>
       </c>
       <c r="J129" t="s" s="2">
-        <v>470</v>
+        <v>548</v>
       </c>
       <c r="K129" t="s" s="2">
-        <v>532</v>
+        <v>549</v>
       </c>
       <c r="L129" t="s" s="2">
-        <v>533</v>
-      </c>
-      <c r="M129" t="s" s="2">
-        <v>534</v>
-      </c>
+        <v>550</v>
+      </c>
+      <c r="M129" s="2"/>
       <c r="N129" s="2"/>
       <c r="O129" t="s" s="2">
         <v>76</v>
@@ -17197,7 +17175,7 @@
         <v>76</v>
       </c>
       <c r="AE129" t="s" s="2">
-        <v>531</v>
+        <v>547</v>
       </c>
       <c r="AF129" t="s" s="2">
         <v>77</v>
@@ -17209,725 +17187,29 @@
         <v>76</v>
       </c>
       <c r="AI129" t="s" s="2">
-        <v>535</v>
+        <v>99</v>
       </c>
       <c r="AJ129" t="s" s="2">
-        <v>76</v>
+        <v>551</v>
       </c>
       <c r="AK129" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL129" t="s" s="2">
-        <v>76</v>
+        <v>552</v>
       </c>
       <c r="AM129" t="s" s="2">
-        <v>536</v>
+        <v>553</v>
       </c>
       <c r="AN129" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AO129" t="s" s="2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="130" hidden="true">
-      <c r="A130" t="s" s="2">
-        <v>537</v>
-      </c>
-      <c r="B130" s="2"/>
-      <c r="C130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="D130" s="2"/>
-      <c r="E130" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="F130" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="G130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="H130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J130" t="s" s="2">
-        <v>89</v>
-      </c>
-      <c r="K130" t="s" s="2">
-        <v>154</v>
-      </c>
-      <c r="L130" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="M130" s="2"/>
-      <c r="N130" s="2"/>
-      <c r="O130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="P130" s="2"/>
-      <c r="Q130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="R130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="S130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Z130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE130" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="AF130" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AG130" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AH130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AI130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AJ130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AK130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AL130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AM130" t="s" s="2">
-        <v>157</v>
-      </c>
-      <c r="AN130" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AO130" t="s" s="2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="131" hidden="true">
-      <c r="A131" t="s" s="2">
-        <v>538</v>
-      </c>
-      <c r="B131" s="2"/>
-      <c r="C131" t="s" s="2">
-        <v>132</v>
-      </c>
-      <c r="D131" s="2"/>
-      <c r="E131" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="F131" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="H131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J131" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="K131" t="s" s="2">
-        <v>134</v>
-      </c>
-      <c r="L131" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="M131" t="s" s="2">
-        <v>136</v>
-      </c>
-      <c r="N131" s="2"/>
-      <c r="O131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="P131" s="2"/>
-      <c r="Q131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="R131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="S131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Z131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE131" t="s" s="2">
-        <v>163</v>
-      </c>
-      <c r="AF131" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AG131" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AI131" t="s" s="2">
-        <v>138</v>
-      </c>
-      <c r="AJ131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AK131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AL131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AM131" t="s" s="2">
-        <v>157</v>
-      </c>
-      <c r="AN131" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AO131" t="s" s="2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="132" hidden="true">
-      <c r="A132" t="s" s="2">
-        <v>539</v>
-      </c>
-      <c r="B132" s="2"/>
-      <c r="C132" t="s" s="2">
-        <v>478</v>
-      </c>
-      <c r="D132" s="2"/>
-      <c r="E132" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="F132" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G132" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="H132" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="I132" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="J132" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="K132" t="s" s="2">
-        <v>479</v>
-      </c>
-      <c r="L132" t="s" s="2">
-        <v>480</v>
-      </c>
-      <c r="M132" t="s" s="2">
-        <v>136</v>
-      </c>
-      <c r="N132" t="s" s="2">
-        <v>142</v>
-      </c>
-      <c r="O132" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="P132" s="2"/>
-      <c r="Q132" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="R132" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="S132" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T132" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U132" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V132" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W132" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X132" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y132" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Z132" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA132" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB132" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC132" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD132" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE132" t="s" s="2">
-        <v>481</v>
-      </c>
-      <c r="AF132" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AG132" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH132" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AI132" t="s" s="2">
-        <v>138</v>
-      </c>
-      <c r="AJ132" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AK132" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AL132" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AM132" t="s" s="2">
-        <v>130</v>
-      </c>
-      <c r="AN132" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AO132" t="s" s="2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="133" hidden="true">
-      <c r="A133" t="s" s="2">
-        <v>540</v>
-      </c>
-      <c r="B133" s="2"/>
-      <c r="C133" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="D133" s="2"/>
-      <c r="E133" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="F133" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G133" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="H133" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I133" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="J133" t="s" s="2">
-        <v>175</v>
-      </c>
-      <c r="K133" t="s" s="2">
-        <v>541</v>
-      </c>
-      <c r="L133" t="s" s="2">
-        <v>542</v>
-      </c>
-      <c r="M133" s="2"/>
-      <c r="N133" s="2"/>
-      <c r="O133" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="P133" s="2"/>
-      <c r="Q133" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="R133" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="S133" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T133" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U133" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V133" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W133" t="s" s="2">
-        <v>348</v>
-      </c>
-      <c r="X133" t="s" s="2">
-        <v>543</v>
-      </c>
-      <c r="Y133" t="s" s="2">
-        <v>544</v>
-      </c>
-      <c r="Z133" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA133" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB133" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC133" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD133" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE133" t="s" s="2">
-        <v>540</v>
-      </c>
-      <c r="AF133" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AG133" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH133" t="s" s="2">
-        <v>545</v>
-      </c>
-      <c r="AI133" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AJ133" t="s" s="2">
-        <v>546</v>
-      </c>
-      <c r="AK133" t="s" s="2">
-        <v>317</v>
-      </c>
-      <c r="AL133" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AM133" t="s" s="2">
-        <v>547</v>
-      </c>
-      <c r="AN133" t="s" s="2">
-        <v>548</v>
-      </c>
-      <c r="AO133" t="s" s="2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="134" hidden="true">
-      <c r="A134" t="s" s="2">
-        <v>549</v>
-      </c>
-      <c r="B134" s="2"/>
-      <c r="C134" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="D134" s="2"/>
-      <c r="E134" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="F134" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G134" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="H134" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I134" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="J134" t="s" s="2">
-        <v>550</v>
-      </c>
-      <c r="K134" t="s" s="2">
-        <v>551</v>
-      </c>
-      <c r="L134" t="s" s="2">
-        <v>552</v>
-      </c>
-      <c r="M134" s="2"/>
-      <c r="N134" s="2"/>
-      <c r="O134" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="P134" s="2"/>
-      <c r="Q134" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="R134" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="S134" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T134" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U134" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V134" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W134" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X134" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y134" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Z134" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA134" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB134" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC134" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD134" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE134" t="s" s="2">
-        <v>549</v>
-      </c>
-      <c r="AF134" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AG134" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH134" t="s" s="2">
-        <v>545</v>
-      </c>
-      <c r="AI134" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AJ134" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AK134" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AL134" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AM134" t="s" s="2">
-        <v>504</v>
-      </c>
-      <c r="AN134" t="s" s="2">
-        <v>548</v>
-      </c>
-      <c r="AO134" t="s" s="2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="135" hidden="true">
-      <c r="A135" t="s" s="2">
-        <v>553</v>
-      </c>
-      <c r="B135" s="2"/>
-      <c r="C135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="D135" s="2"/>
-      <c r="E135" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="F135" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="H135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J135" t="s" s="2">
-        <v>554</v>
-      </c>
-      <c r="K135" t="s" s="2">
-        <v>555</v>
-      </c>
-      <c r="L135" t="s" s="2">
-        <v>556</v>
-      </c>
-      <c r="M135" s="2"/>
-      <c r="N135" s="2"/>
-      <c r="O135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="P135" s="2"/>
-      <c r="Q135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="R135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="S135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Z135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE135" t="s" s="2">
-        <v>553</v>
-      </c>
-      <c r="AF135" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AG135" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AI135" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AJ135" t="s" s="2">
-        <v>557</v>
-      </c>
-      <c r="AK135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AL135" t="s" s="2">
-        <v>558</v>
-      </c>
-      <c r="AM135" t="s" s="2">
-        <v>559</v>
-      </c>
-      <c r="AN135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AO135" t="s" s="2">
         <v>76</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO135">
+  <autoFilter ref="A1:AO129">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -17937,7 +17219,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI134">
+  <conditionalFormatting sqref="A2:AI128">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>